<commit_message>
DOCS: Fix some cell value error of 'PX4-Autopilot_CWE_result_analysis.xlsx'
</commit_message>
<xml_diff>
--- a/static_analysis/codeql/PX4-Autopilot/PX4-Autopilot_CWE_result_analysis.xlsx
+++ b/static_analysis/codeql/PX4-Autopilot/PX4-Autopilot_CWE_result_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folder\대학\2024_A(4-1)\CapstoneDesign\CD_repo\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BCE75F-480B-45B9-8E22-90ED1B3C35CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A227E52-50E6-4517-BEAF-17023F462176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="337">
   <si>
     <t>Uncontrolled data used in path expression</t>
   </si>
@@ -1064,10 +1064,6 @@
   </si>
   <si>
     <t>Value Overflow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Else</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -2391,7 +2387,7 @@
     </row>
     <row r="8" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C8" t="s">
         <v>327</v>
@@ -2531,7 +2527,7 @@
     </row>
     <row r="12" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C12" t="s">
         <v>327</v>
@@ -2671,7 +2667,7 @@
     </row>
     <row r="16" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C16" t="s">
         <v>327</v>
@@ -2776,7 +2772,7 @@
     </row>
     <row r="19" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C19" t="s">
         <v>327</v>
@@ -2811,7 +2807,7 @@
     </row>
     <row r="20" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C20" t="s">
         <v>328</v>
@@ -2881,7 +2877,7 @@
     </row>
     <row r="22" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C22" t="s">
         <v>327</v>
@@ -3826,7 +3822,7 @@
     </row>
     <row r="49" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C49" t="s">
         <v>327</v>
@@ -3861,7 +3857,7 @@
     </row>
     <row r="50" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C50" t="s">
         <v>327</v>
@@ -3896,7 +3892,7 @@
     </row>
     <row r="51" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B51" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C51" t="s">
         <v>328</v>
@@ -3931,7 +3927,7 @@
     </row>
     <row r="52" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C52" t="s">
         <v>328</v>
@@ -3966,7 +3962,7 @@
     </row>
     <row r="53" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C53" t="s">
         <v>327</v>
@@ -5191,7 +5187,7 @@
     </row>
     <row r="88" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B88" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C88" t="s">
         <v>327</v>
@@ -6469,7 +6465,7 @@
         <v>78</v>
       </c>
       <c r="H124" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I124">
         <v>208</v>
@@ -6731,7 +6727,7 @@
     </row>
     <row r="132" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B132" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C132" t="s">
         <v>327</v>
@@ -7011,7 +7007,7 @@
     </row>
     <row r="140" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B140" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C140" t="s">
         <v>327</v>
@@ -7186,7 +7182,7 @@
     </row>
     <row r="145" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B145" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C145" t="s">
         <v>327</v>
@@ -7571,7 +7567,7 @@
     </row>
     <row r="156" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B156" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C156" t="s">
         <v>327</v>
@@ -7606,7 +7602,7 @@
     </row>
     <row r="157" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B157" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C157" t="s">
         <v>327</v>
@@ -7676,7 +7672,7 @@
     </row>
     <row r="159" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B159" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C159" t="s">
         <v>327</v>
@@ -8131,7 +8127,7 @@
     </row>
     <row r="172" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B172" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C172" t="s">
         <v>327</v>
@@ -8166,7 +8162,7 @@
     </row>
     <row r="173" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B173" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C173" t="s">
         <v>328</v>
@@ -8201,7 +8197,7 @@
     </row>
     <row r="174" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B174" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C174" t="s">
         <v>328</v>
@@ -10091,7 +10087,7 @@
     </row>
     <row r="228" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B228" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C228" t="s">
         <v>327</v>

</xml_diff>

<commit_message>
DOCS: Update CWE result analysis file
</commit_message>
<xml_diff>
--- a/static_analysis/codeql/PX4-Autopilot/PX4-Autopilot_CWE_result_analysis.xlsx
+++ b/static_analysis/codeql/PX4-Autopilot/PX4-Autopilot_CWE_result_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr showObjects="none" codeName="현재_통합_문서" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folder\대학\2024_A(4-1)\CapstoneDesign\CD_repo\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A227E52-50E6-4517-BEAF-17023F462176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB30AD4E-915D-4655-A180-DE4576941F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="790" yWindow="670" windowWidth="27800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PX4-Autopilot_CWE_result" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1887" uniqueCount="365">
   <si>
     <t>Uncontrolled data used in path expression</t>
   </si>
@@ -1080,6 +1080,118 @@
   </si>
   <si>
     <t>/src/modules/load_mon/LoadMon.cpp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vulnerability analysis result</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Analysis detail</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seems safe</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Possibility, but work as intended</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PX4의 초기화 스크립트 구조 상 main의 인수로 파일명을 받아서 스크립트를 실행시킬 수 있음</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cannot confirm</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Highly safe</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>recommendation</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PX4의 MAVLink module이 값을 읽어서 MAVLink github 저장소를 빌드한 헤더에서 산술 오버플로우가 날 수 있다는 경고이지만, 정확한 분석이 어려움. 조사 필요.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>probably safe</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PX4의 MAVLink module이 값을 읽어서 MAVLink github 저장소를 빌드한 헤더에서 산술 오버플로우가 날 수 있다는 경고이지만/ 정확한 분석이 어려움. 조사 필요.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>main 인수로 instance id 설정하는 부분. 적절한 값을 넣으면 instance id가 특정 값이나 음수가 될 수 있고/ SITL에서 0번 등 임의의 port로 MAVLink를 여는 등의 동작이 이루어지는 것을 확인/ 취약점 사용 여지는 조사 필요.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0666 권한으로 만든 파일은 lock 파일으로/ PX4 server 혹은 client 프로세스 간 동기화를 위해 사용하는것으로 추정. 취약점 사용 여지는 조사 필요.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>String length is checked at line 483. If 'kMaxDataLength' has proper value.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>strncpy로 인한 쓰기 동작이 버퍼의 크기를 넘어가지 않음. Source 버퍼의 크기가 작아서 잘못된 사용이라고 CodeQL에서 "recommendation" 수준으로 경고하지만/ 크기가 작아도 NULL 문자만 destination 버퍼에 허용된 길이 만큼 쓰임. 전처리기 매크로로 인하여 source 버퍼의 크기가 달라질 수 있는데 CodeQL은 이를 확인하지 못 하기 때문에 항상 1~2바이트인 것으로 판정하였음.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAVLink FTP가 파일을 복사할 때 0666 권한을 지정하는 구문이지만/ 전처리기 구문을 통해 POSIX 환경에 한정한 권한이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>정확히는 사용자 입력이 아니고 로그 관련 파일을 열어서 그 파일 안의 내용을 읽어 필요한 로그 파일명을 얻고/ 그 로그 파일들을 다시 열어서 외부로? 전송하는 내용으로 대략적으로 분석하였다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>코드 상에서 파일을 열어서 하는 동작은 CRC 검사이고/ ftp를 위해 파일을 여는 것은 공격자가 의도한 파일(설정 등)을 열어서 프로그램의 동작을 변경시키는 것과 관계가 없다고 추정함.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>new'를 통한 할당이 NULL 포인터를 리턴하였는지 점검하는 구문에서/ 이 'new'는 NULL 포인터가 아니라 예외를 던지므로 잘못된 점검이라는 경고. 예외가 발생한 경우 제대로 처리되는지는 코드상에서 좀 더 확인이 필요하지만/ 예외가 처리되지 않아서 해결할 수 없는 메모리 부족 문제는 프로그램 종료로 이어지며 이는 어쩔 수 없는 일반적인 동작. 실제 하드웨어에서 메모리 부족이 일어날 수 있는 가능성이나 이로 인한 문제는 조사가 필요하며/ 환경에 따라서 'new'를 통한 할당이 std::nothrow를 사용하지 않아도 NULL 포인터를 리턴하는 경우가 있으므로/ 점검 구문 자체는 있어서 문제가 되지 않는다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Surely weakness, but bare possibility</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>px4_clock_gettime은 posix 환경에서 결국 clock_gettime으로 이어지고/ 코드에서는 이 함수의 리턴값을 점검하지 않았으므로/ 스택에 있는 내용을 잘못된 시간값으로 읽어서 MAVLink를 통해 전송할 가능성이 존재함. 다만 clock_gettime이 실패할 가능성은 거의 없다고 보여짐.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>"_external_mode_names[idx].name"의 값은 다른 곳에서 읽어와서 설정이 되는데/ 이것이 NULL 문자로 끝나는 것을 보장한다면 문제가 없음. 실제로 보장하는지는 확인이 필요함.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Surely safe</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격자가 코드에서 읽어오는 로그 관련 파일을 수정할 수 있다면/ 해당 파일에서 로그 파일명을 읽어오는 과정에서 스택 overflow가 발생 가능한 것으로 보였으나 fgets 에서 문자열 길이가 차단됨.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Possibility, but need more analysis</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그 파일을 편의를 위해 하나로 합칠 때 해당 권한이 0666인 문제. 이를 공격자가 조작하여 원하는 파일을 QGroundControl로 받아올 수 있는 것을 확인.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vulnerability, tested</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1673,8 +1785,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1722,7 +1837,13 @@
     <cellStyle name="출력" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="15">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1776,26 +1897,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B99CD39-F295-4560-994D-36C3706EB741}" name="표1" displayName="표1" ref="A1:L229" totalsRowCount="1" dataDxfId="12">
-  <autoFilter ref="A1:L228" xr:uid="{3B99CD39-F295-4560-994D-36C3706EB741}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B99CD39-F295-4560-994D-36C3706EB741}" name="표1" displayName="표1" ref="A1:N229" totalsRowCount="1" dataDxfId="14">
+  <autoFilter ref="A1:N228" xr:uid="{3B99CD39-F295-4560-994D-36C3706EB741}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:L228">
     <sortCondition ref="H1:H228"/>
   </sortState>
-  <tableColumns count="12">
-    <tableColumn id="10" xr3:uid="{9D8022D2-0396-4EA6-BCB2-B2F62285DA6D}" name="열1" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{D79EC2A5-7CD8-43BC-912D-5C1CDAFE163D}" name="Type" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{AAB300F3-1C76-441D-BAD5-7E6D2FD21449}" name="유사성 필터" totalsRowFunction="custom" dataDxfId="9">
+  <tableColumns count="14">
+    <tableColumn id="10" xr3:uid="{9D8022D2-0396-4EA6-BCB2-B2F62285DA6D}" name="열1" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{D79EC2A5-7CD8-43BC-912D-5C1CDAFE163D}" name="Type" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{AAB300F3-1C76-441D-BAD5-7E6D2FD21449}" name="유사성 필터" totalsRowFunction="custom" dataDxfId="11">
       <totalsRowFormula>_xlfn.CONCAT("필터링된 수: ",TEXT(SUBTOTAL(103,C$2:C228),0))</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{EC3DE87F-2CA0-4424-991A-A8D8F98049B1}" name="CWE Type" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{EC3FF5A7-A0FC-445A-97EE-E8F890A34601}" name="CWE Type Description" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{727A2C73-6D52-46B9-8770-2CE8FF74323D}" name="CWE Level" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{F2437DC5-713E-4987-9BAB-DC77402C1224}" name="Detail &amp; position of cause" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{62B54862-4EEE-49F5-AC8F-507557C1EBBC}" name="Filename" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{50BE20C8-1E8C-445D-AEF3-80B52D747875}" name="StartLine" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{DCB91EC0-95A2-4F94-A2BE-8BC3324ACC42}" name="StartColumn" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{AC9542A5-BA04-4537-9A46-41055DB133E2}" name="EndLine" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00C4581C-9B5B-4A43-A6E2-24348E1AD267}" name="EndColumn" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{EC3DE87F-2CA0-4424-991A-A8D8F98049B1}" name="CWE Type" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{EC3FF5A7-A0FC-445A-97EE-E8F890A34601}" name="CWE Type Description" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{727A2C73-6D52-46B9-8770-2CE8FF74323D}" name="CWE Level" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{F2437DC5-713E-4987-9BAB-DC77402C1224}" name="Detail &amp; position of cause" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{62B54862-4EEE-49F5-AC8F-507557C1EBBC}" name="Filename" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{50BE20C8-1E8C-445D-AEF3-80B52D747875}" name="StartLine" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{DCB91EC0-95A2-4F94-A2BE-8BC3324ACC42}" name="StartColumn" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{AC9542A5-BA04-4537-9A46-41055DB133E2}" name="EndLine" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00C4581C-9B5B-4A43-A6E2-24348E1AD267}" name="EndColumn" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{2EEA516E-A3F5-4CF9-B324-ADC62F867E03}" name="Vulnerability analysis result" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{E049123C-DBF2-40F6-BCC2-4144A0E4106A}" name="Analysis detail" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2119,10 +2242,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L229"/>
+  <dimension ref="A1:N229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2130,14 +2253,18 @@
     <col min="1" max="1" width="9.58203125" customWidth="1"/>
     <col min="2" max="2" width="20.58203125" customWidth="1"/>
     <col min="3" max="3" width="17.25" customWidth="1"/>
-    <col min="4" max="5" width="40.58203125" customWidth="1"/>
-    <col min="6" max="6" width="12.58203125" customWidth="1"/>
-    <col min="7" max="7" width="40.58203125" customWidth="1"/>
-    <col min="8" max="8" width="46.9140625" customWidth="1"/>
-    <col min="9" max="12" width="12.58203125" customWidth="1"/>
+    <col min="4" max="4" width="2.58203125" customWidth="1"/>
+    <col min="5" max="5" width="23.4140625" customWidth="1"/>
+    <col min="6" max="6" width="1.08203125" customWidth="1"/>
+    <col min="7" max="7" width="19.4140625" customWidth="1"/>
+    <col min="8" max="8" width="48.5" customWidth="1"/>
+    <col min="9" max="9" width="12.58203125" customWidth="1"/>
+    <col min="10" max="12" width="12.58203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="28.9140625" customWidth="1"/>
+    <col min="14" max="14" width="40.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>321</v>
       </c>
@@ -2174,8 +2301,14 @@
       <c r="L1" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M1" t="s">
+        <v>337</v>
+      </c>
+      <c r="N1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>332</v>
       </c>
@@ -2209,8 +2342,14 @@
       <c r="L2">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M2" t="s">
+        <v>342</v>
+      </c>
+      <c r="N2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>332</v>
       </c>
@@ -2244,8 +2383,14 @@
       <c r="L3">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M3" t="s">
+        <v>345</v>
+      </c>
+      <c r="N3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>332</v>
       </c>
@@ -2279,8 +2424,14 @@
       <c r="L4">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M4" t="s">
+        <v>345</v>
+      </c>
+      <c r="N4" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>332</v>
       </c>
@@ -2314,8 +2465,14 @@
       <c r="L5">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M5" t="s">
+        <v>345</v>
+      </c>
+      <c r="N5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>332</v>
       </c>
@@ -2349,8 +2506,14 @@
       <c r="L6">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M6" t="s">
+        <v>345</v>
+      </c>
+      <c r="N6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>332</v>
       </c>
@@ -2384,8 +2547,14 @@
       <c r="L7">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M7" t="s">
+        <v>345</v>
+      </c>
+      <c r="N7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>333</v>
       </c>
@@ -2420,7 +2589,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>333</v>
       </c>
@@ -2455,7 +2624,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>331</v>
       </c>
@@ -2490,7 +2659,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>331</v>
       </c>
@@ -2524,8 +2693,14 @@
       <c r="L11">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M11" t="s">
+        <v>342</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>335</v>
       </c>
@@ -2560,7 +2735,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>331</v>
       </c>
@@ -2594,8 +2769,14 @@
       <c r="L13">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M13" t="s">
+        <v>342</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>331</v>
       </c>
@@ -2629,8 +2810,14 @@
       <c r="L14">
         <v>74</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M14" t="s">
+        <v>342</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>331</v>
       </c>
@@ -2664,8 +2851,14 @@
       <c r="L15">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M15" t="s">
+        <v>342</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>334</v>
       </c>
@@ -2699,8 +2892,14 @@
       <c r="L16">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M16" t="s">
+        <v>340</v>
+      </c>
+      <c r="N16" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>332</v>
       </c>
@@ -2734,8 +2933,14 @@
       <c r="L17">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M17" t="s">
+        <v>362</v>
+      </c>
+      <c r="N17" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>332</v>
       </c>
@@ -2769,8 +2974,14 @@
       <c r="L18">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M18" t="s">
+        <v>342</v>
+      </c>
+      <c r="N18" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>335</v>
       </c>
@@ -2804,8 +3015,14 @@
       <c r="L19">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M19" t="s">
+        <v>362</v>
+      </c>
+      <c r="N19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>335</v>
       </c>
@@ -2839,8 +3056,14 @@
       <c r="L20">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M20" t="s">
+        <v>342</v>
+      </c>
+      <c r="N20" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>332</v>
       </c>
@@ -2875,7 +3098,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>333</v>
       </c>
@@ -2910,7 +3133,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>333</v>
       </c>
@@ -2945,7 +3168,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>333</v>
       </c>
@@ -2980,7 +3203,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>333</v>
       </c>
@@ -3015,7 +3238,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>333</v>
       </c>
@@ -3050,7 +3273,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>331</v>
       </c>
@@ -3084,8 +3307,14 @@
       <c r="L27">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M27" t="s">
+        <v>342</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>332</v>
       </c>
@@ -3120,7 +3349,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>331</v>
       </c>
@@ -3154,8 +3383,14 @@
       <c r="L29">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M29" t="s">
+        <v>342</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>330</v>
       </c>
@@ -3190,7 +3425,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>330</v>
       </c>
@@ -3225,7 +3460,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>330</v>
       </c>
@@ -3260,7 +3495,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>330</v>
       </c>
@@ -3295,7 +3530,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>331</v>
       </c>
@@ -3330,7 +3565,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>331</v>
       </c>
@@ -3364,8 +3599,14 @@
       <c r="L35">
         <v>37</v>
       </c>
-    </row>
-    <row r="36" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M35" t="s">
+        <v>342</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
         <v>331</v>
       </c>
@@ -3399,8 +3640,14 @@
       <c r="L36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M36" t="s">
+        <v>342</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
         <v>331</v>
       </c>
@@ -3434,8 +3681,14 @@
       <c r="L37">
         <v>38</v>
       </c>
-    </row>
-    <row r="38" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M37" t="s">
+        <v>342</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
         <v>331</v>
       </c>
@@ -3469,8 +3722,14 @@
       <c r="L38">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M38" t="s">
+        <v>342</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
         <v>331</v>
       </c>
@@ -3504,8 +3763,14 @@
       <c r="L39">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M39" t="s">
+        <v>342</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
         <v>331</v>
       </c>
@@ -3539,8 +3804,14 @@
       <c r="L40">
         <v>34</v>
       </c>
-    </row>
-    <row r="41" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M40" t="s">
+        <v>342</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
         <v>331</v>
       </c>
@@ -3574,8 +3845,14 @@
       <c r="L41">
         <v>52</v>
       </c>
-    </row>
-    <row r="42" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M41" t="s">
+        <v>342</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>331</v>
       </c>
@@ -3609,8 +3886,14 @@
       <c r="L42">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M42" t="s">
+        <v>342</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
         <v>332</v>
       </c>
@@ -3645,7 +3928,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
         <v>331</v>
       </c>
@@ -3679,8 +3962,14 @@
       <c r="L44">
         <v>75</v>
       </c>
-    </row>
-    <row r="45" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M44" t="s">
+        <v>342</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
         <v>331</v>
       </c>
@@ -3715,7 +4004,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
         <v>331</v>
       </c>
@@ -3749,8 +4038,14 @@
       <c r="L46">
         <v>23</v>
       </c>
-    </row>
-    <row r="47" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M46" t="s">
+        <v>342</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
         <v>331</v>
       </c>
@@ -3784,8 +4079,14 @@
       <c r="L47">
         <v>41</v>
       </c>
-    </row>
-    <row r="48" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M47" t="s">
+        <v>342</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" t="s">
         <v>331</v>
       </c>
@@ -3818,6 +4119,12 @@
       </c>
       <c r="L48">
         <v>32</v>
+      </c>
+      <c r="M48" t="s">
+        <v>342</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="49" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
@@ -4380,7 +4687,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
         <v>330</v>
       </c>
@@ -4415,7 +4722,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
         <v>330</v>
       </c>
@@ -4450,7 +4757,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B67" t="s">
         <v>332</v>
       </c>
@@ -4485,7 +4792,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B68" t="s">
         <v>332</v>
       </c>
@@ -4520,7 +4827,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B69" t="s">
         <v>332</v>
       </c>
@@ -4555,7 +4862,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B70" t="s">
         <v>332</v>
       </c>
@@ -4590,7 +4897,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B71" t="s">
         <v>332</v>
       </c>
@@ -4625,7 +4932,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B72" t="s">
         <v>332</v>
       </c>
@@ -4660,7 +4967,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B73" t="s">
         <v>332</v>
       </c>
@@ -4695,7 +5002,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B74" t="s">
         <v>332</v>
       </c>
@@ -4730,7 +5037,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B75" t="s">
         <v>332</v>
       </c>
@@ -4765,7 +5072,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B76" t="s">
         <v>332</v>
       </c>
@@ -4800,7 +5107,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B77" t="s">
         <v>332</v>
       </c>
@@ -4835,7 +5142,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="78" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B78" t="s">
         <v>332</v>
       </c>
@@ -4870,7 +5177,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B79" t="s">
         <v>331</v>
       </c>
@@ -4904,8 +5211,14 @@
       <c r="L79">
         <v>64</v>
       </c>
-    </row>
-    <row r="80" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M79" t="s">
+        <v>342</v>
+      </c>
+      <c r="N79" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="80" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B80" t="s">
         <v>331</v>
       </c>
@@ -4939,8 +5252,14 @@
       <c r="L80">
         <v>43</v>
       </c>
-    </row>
-    <row r="81" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M80" t="s">
+        <v>342</v>
+      </c>
+      <c r="N80" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="81" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B81" t="s">
         <v>331</v>
       </c>
@@ -4974,8 +5293,14 @@
       <c r="L81">
         <v>56</v>
       </c>
-    </row>
-    <row r="82" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M81" t="s">
+        <v>342</v>
+      </c>
+      <c r="N81" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="82" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B82" t="s">
         <v>331</v>
       </c>
@@ -5009,8 +5334,14 @@
       <c r="L82">
         <v>48</v>
       </c>
-    </row>
-    <row r="83" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M82" t="s">
+        <v>342</v>
+      </c>
+      <c r="N82" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="83" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B83" t="s">
         <v>331</v>
       </c>
@@ -5044,8 +5375,14 @@
       <c r="L83">
         <v>38</v>
       </c>
-    </row>
-    <row r="84" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M83" t="s">
+        <v>342</v>
+      </c>
+      <c r="N83" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="84" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B84" t="s">
         <v>332</v>
       </c>
@@ -5080,7 +5417,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="85" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B85" t="s">
         <v>332</v>
       </c>
@@ -5115,7 +5452,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="86" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B86" t="s">
         <v>332</v>
       </c>
@@ -5150,7 +5487,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B87" t="s">
         <v>331</v>
       </c>
@@ -5184,8 +5521,14 @@
       <c r="L87">
         <v>52</v>
       </c>
-    </row>
-    <row r="88" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M87" t="s">
+        <v>342</v>
+      </c>
+      <c r="N87" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="88" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B88" t="s">
         <v>335</v>
       </c>
@@ -5220,7 +5563,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="89" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B89" t="s">
         <v>331</v>
       </c>
@@ -5254,8 +5597,14 @@
       <c r="L89">
         <v>54</v>
       </c>
-    </row>
-    <row r="90" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M89" t="s">
+        <v>342</v>
+      </c>
+      <c r="N89" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="90" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B90" t="s">
         <v>331</v>
       </c>
@@ -5289,8 +5638,14 @@
       <c r="L90">
         <v>64</v>
       </c>
-    </row>
-    <row r="91" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M90" t="s">
+        <v>342</v>
+      </c>
+      <c r="N90" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="91" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B91" t="s">
         <v>331</v>
       </c>
@@ -5324,8 +5679,14 @@
       <c r="L91">
         <v>76</v>
       </c>
-    </row>
-    <row r="92" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M91" t="s">
+        <v>342</v>
+      </c>
+      <c r="N91" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="92" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B92" t="s">
         <v>331</v>
       </c>
@@ -5359,8 +5720,14 @@
       <c r="L92">
         <v>67</v>
       </c>
-    </row>
-    <row r="93" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M92" t="s">
+        <v>342</v>
+      </c>
+      <c r="N92" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="93" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B93" t="s">
         <v>331</v>
       </c>
@@ -5394,8 +5761,14 @@
       <c r="L93">
         <v>74</v>
       </c>
-    </row>
-    <row r="94" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M93" t="s">
+        <v>342</v>
+      </c>
+      <c r="N93" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="94" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B94" t="s">
         <v>331</v>
       </c>
@@ -5429,8 +5802,14 @@
       <c r="L94">
         <v>63</v>
       </c>
-    </row>
-    <row r="95" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M94" t="s">
+        <v>342</v>
+      </c>
+      <c r="N94" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="95" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B95" t="s">
         <v>331</v>
       </c>
@@ -5464,8 +5843,14 @@
       <c r="L95">
         <v>65</v>
       </c>
-    </row>
-    <row r="96" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M95" t="s">
+        <v>342</v>
+      </c>
+      <c r="N95" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="96" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B96" t="s">
         <v>331</v>
       </c>
@@ -5499,8 +5884,14 @@
       <c r="L96">
         <v>71</v>
       </c>
-    </row>
-    <row r="97" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M96" t="s">
+        <v>342</v>
+      </c>
+      <c r="N96" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="97" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B97" t="s">
         <v>331</v>
       </c>
@@ -5534,8 +5925,14 @@
       <c r="L97">
         <v>63</v>
       </c>
-    </row>
-    <row r="98" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M97" t="s">
+        <v>342</v>
+      </c>
+      <c r="N97" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="98" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B98" t="s">
         <v>331</v>
       </c>
@@ -5569,8 +5966,14 @@
       <c r="L98">
         <v>61</v>
       </c>
-    </row>
-    <row r="99" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M98" t="s">
+        <v>342</v>
+      </c>
+      <c r="N98" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="99" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
         <v>331</v>
       </c>
@@ -5604,8 +6007,14 @@
       <c r="L99">
         <v>62</v>
       </c>
-    </row>
-    <row r="100" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M99" t="s">
+        <v>342</v>
+      </c>
+      <c r="N99" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="100" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B100" t="s">
         <v>331</v>
       </c>
@@ -5639,8 +6048,14 @@
       <c r="L100">
         <v>34</v>
       </c>
-    </row>
-    <row r="101" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M100" t="s">
+        <v>342</v>
+      </c>
+      <c r="N100" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="101" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B101" t="s">
         <v>332</v>
       </c>
@@ -5675,7 +6090,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="102" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B102" t="s">
         <v>332</v>
       </c>
@@ -5710,7 +6125,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="103" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B103" t="s">
         <v>331</v>
       </c>
@@ -5744,8 +6159,14 @@
       <c r="L103">
         <v>42</v>
       </c>
-    </row>
-    <row r="104" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M103" t="s">
+        <v>342</v>
+      </c>
+      <c r="N103" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="104" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B104" t="s">
         <v>331</v>
       </c>
@@ -5779,8 +6200,14 @@
       <c r="L104">
         <v>76</v>
       </c>
-    </row>
-    <row r="105" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M104" t="s">
+        <v>342</v>
+      </c>
+      <c r="N104" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="105" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B105" t="s">
         <v>331</v>
       </c>
@@ -5814,8 +6241,14 @@
       <c r="L105">
         <v>78</v>
       </c>
-    </row>
-    <row r="106" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M105" t="s">
+        <v>342</v>
+      </c>
+      <c r="N105" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="106" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B106" t="s">
         <v>331</v>
       </c>
@@ -5849,8 +6282,14 @@
       <c r="L106">
         <v>40</v>
       </c>
-    </row>
-    <row r="107" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M106" t="s">
+        <v>342</v>
+      </c>
+      <c r="N106" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="107" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B107" t="s">
         <v>331</v>
       </c>
@@ -5884,8 +6323,14 @@
       <c r="L107">
         <v>54</v>
       </c>
-    </row>
-    <row r="108" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M107" t="s">
+        <v>342</v>
+      </c>
+      <c r="N107" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="108" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B108" t="s">
         <v>331</v>
       </c>
@@ -5919,8 +6364,14 @@
       <c r="L108">
         <v>72</v>
       </c>
-    </row>
-    <row r="109" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M108" t="s">
+        <v>342</v>
+      </c>
+      <c r="N108" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="109" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B109" t="s">
         <v>331</v>
       </c>
@@ -5954,8 +6405,14 @@
       <c r="L109">
         <v>77</v>
       </c>
-    </row>
-    <row r="110" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M109" t="s">
+        <v>342</v>
+      </c>
+      <c r="N109" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="110" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B110" t="s">
         <v>331</v>
       </c>
@@ -5989,8 +6446,14 @@
       <c r="L110">
         <v>72</v>
       </c>
-    </row>
-    <row r="111" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M110" t="s">
+        <v>342</v>
+      </c>
+      <c r="N110" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="111" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B111" t="s">
         <v>331</v>
       </c>
@@ -6024,8 +6487,14 @@
       <c r="L111">
         <v>64</v>
       </c>
-    </row>
-    <row r="112" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M111" t="s">
+        <v>342</v>
+      </c>
+      <c r="N111" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="112" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B112" t="s">
         <v>331</v>
       </c>
@@ -6059,8 +6528,14 @@
       <c r="L112">
         <v>47</v>
       </c>
-    </row>
-    <row r="113" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M112" t="s">
+        <v>342</v>
+      </c>
+      <c r="N112" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="113" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B113" t="s">
         <v>331</v>
       </c>
@@ -6094,8 +6569,14 @@
       <c r="L113">
         <v>54</v>
       </c>
-    </row>
-    <row r="114" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M113" t="s">
+        <v>342</v>
+      </c>
+      <c r="N113" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="114" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B114" t="s">
         <v>331</v>
       </c>
@@ -6129,8 +6610,14 @@
       <c r="L114">
         <v>54</v>
       </c>
-    </row>
-    <row r="115" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M114" t="s">
+        <v>342</v>
+      </c>
+      <c r="N114" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="115" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B115" t="s">
         <v>331</v>
       </c>
@@ -6164,8 +6651,14 @@
       <c r="L115">
         <v>50</v>
       </c>
-    </row>
-    <row r="116" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M115" t="s">
+        <v>342</v>
+      </c>
+      <c r="N115" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="116" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B116" t="s">
         <v>332</v>
       </c>
@@ -6200,7 +6693,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="117" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B117" t="s">
         <v>331</v>
       </c>
@@ -6234,8 +6727,14 @@
       <c r="L117">
         <v>34</v>
       </c>
-    </row>
-    <row r="118" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M117" t="s">
+        <v>342</v>
+      </c>
+      <c r="N117" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="118" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B118" t="s">
         <v>331</v>
       </c>
@@ -6269,8 +6768,14 @@
       <c r="L118">
         <v>36</v>
       </c>
-    </row>
-    <row r="119" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M118" t="s">
+        <v>342</v>
+      </c>
+      <c r="N118" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="119" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B119" t="s">
         <v>331</v>
       </c>
@@ -6304,8 +6809,14 @@
       <c r="L119">
         <v>36</v>
       </c>
-    </row>
-    <row r="120" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M119" t="s">
+        <v>342</v>
+      </c>
+      <c r="N119" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="120" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B120" t="s">
         <v>331</v>
       </c>
@@ -6339,8 +6850,14 @@
       <c r="L120">
         <v>36</v>
       </c>
-    </row>
-    <row r="121" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M120" t="s">
+        <v>342</v>
+      </c>
+      <c r="N120" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="121" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B121" t="s">
         <v>331</v>
       </c>
@@ -6374,8 +6891,14 @@
       <c r="L121">
         <v>32</v>
       </c>
-    </row>
-    <row r="122" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M121" t="s">
+        <v>342</v>
+      </c>
+      <c r="N121" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="122" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B122" t="s">
         <v>331</v>
       </c>
@@ -6409,8 +6932,14 @@
       <c r="L122">
         <v>34</v>
       </c>
-    </row>
-    <row r="123" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M122" t="s">
+        <v>342</v>
+      </c>
+      <c r="N122" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="123" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B123" t="s">
         <v>331</v>
       </c>
@@ -6444,8 +6973,14 @@
       <c r="L123">
         <v>39</v>
       </c>
-    </row>
-    <row r="124" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M123" t="s">
+        <v>342</v>
+      </c>
+      <c r="N123" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="124" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B124" t="s">
         <v>332</v>
       </c>
@@ -6480,7 +7015,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="125" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B125" t="s">
         <v>332</v>
       </c>
@@ -6515,7 +7050,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="126" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B126" t="s">
         <v>332</v>
       </c>
@@ -6550,7 +7085,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="127" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B127" t="s">
         <v>332</v>
       </c>
@@ -6585,7 +7120,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="128" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B128" t="s">
         <v>331</v>
       </c>
@@ -6619,8 +7154,14 @@
       <c r="L128">
         <v>29</v>
       </c>
-    </row>
-    <row r="129" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M128" t="s">
+        <v>342</v>
+      </c>
+      <c r="N128" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="129" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B129" t="s">
         <v>331</v>
       </c>
@@ -6654,8 +7195,14 @@
       <c r="L129">
         <v>74</v>
       </c>
-    </row>
-    <row r="130" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M129" t="s">
+        <v>342</v>
+      </c>
+      <c r="N129" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="130" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B130" t="s">
         <v>331</v>
       </c>
@@ -6689,8 +7236,14 @@
       <c r="L130">
         <v>85</v>
       </c>
-    </row>
-    <row r="131" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M130" t="s">
+        <v>342</v>
+      </c>
+      <c r="N130" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="131" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B131" t="s">
         <v>331</v>
       </c>
@@ -6724,8 +7277,14 @@
       <c r="L131">
         <v>78</v>
       </c>
-    </row>
-    <row r="132" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M131" t="s">
+        <v>342</v>
+      </c>
+      <c r="N131" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="132" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B132" t="s">
         <v>335</v>
       </c>
@@ -6760,7 +7319,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="133" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B133" t="s">
         <v>330</v>
       </c>
@@ -6795,7 +7354,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="134" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B134" t="s">
         <v>332</v>
       </c>
@@ -6830,7 +7389,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="135" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B135" t="s">
         <v>332</v>
       </c>
@@ -6865,7 +7424,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="136" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B136" t="s">
         <v>332</v>
       </c>
@@ -6900,7 +7459,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="137" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B137" t="s">
         <v>330</v>
       </c>
@@ -6935,7 +7494,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B138" t="s">
         <v>331</v>
       </c>
@@ -6969,8 +7528,14 @@
       <c r="L138">
         <v>44</v>
       </c>
-    </row>
-    <row r="139" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M138" t="s">
+        <v>342</v>
+      </c>
+      <c r="N138" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="139" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B139" t="s">
         <v>331</v>
       </c>
@@ -7004,8 +7569,14 @@
       <c r="L139">
         <v>20</v>
       </c>
-    </row>
-    <row r="140" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M139" t="s">
+        <v>342</v>
+      </c>
+      <c r="N139" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="140" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B140" t="s">
         <v>335</v>
       </c>
@@ -7040,7 +7611,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="141" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B141" t="s">
         <v>331</v>
       </c>
@@ -7074,8 +7645,14 @@
       <c r="L141">
         <v>21</v>
       </c>
-    </row>
-    <row r="142" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M141" t="s">
+        <v>342</v>
+      </c>
+      <c r="N141" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="142" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B142" t="s">
         <v>331</v>
       </c>
@@ -7109,8 +7686,14 @@
       <c r="L142">
         <v>47</v>
       </c>
-    </row>
-    <row r="143" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M142" t="s">
+        <v>342</v>
+      </c>
+      <c r="N142" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="143" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B143" t="s">
         <v>331</v>
       </c>
@@ -7144,8 +7727,14 @@
       <c r="L143">
         <v>46</v>
       </c>
-    </row>
-    <row r="144" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M143" t="s">
+        <v>342</v>
+      </c>
+      <c r="N143" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="144" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B144" t="s">
         <v>331</v>
       </c>
@@ -7179,8 +7768,14 @@
       <c r="L144">
         <v>31</v>
       </c>
-    </row>
-    <row r="145" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M144" t="s">
+        <v>342</v>
+      </c>
+      <c r="N144" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="145" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B145" t="s">
         <v>334</v>
       </c>
@@ -7214,8 +7809,14 @@
       <c r="L145">
         <v>30</v>
       </c>
-    </row>
-    <row r="146" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M145" t="s">
+        <v>339</v>
+      </c>
+      <c r="N145" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="146" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B146" t="s">
         <v>330</v>
       </c>
@@ -7249,8 +7850,14 @@
       <c r="L146">
         <v>8</v>
       </c>
-    </row>
-    <row r="147" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M146" t="s">
+        <v>339</v>
+      </c>
+      <c r="N146" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="147" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B147" t="s">
         <v>330</v>
       </c>
@@ -7264,7 +7871,7 @@
         <v>23</v>
       </c>
       <c r="F147" t="s">
-        <v>24</v>
+        <v>344</v>
       </c>
       <c r="G147" t="s">
         <v>27</v>
@@ -7284,8 +7891,14 @@
       <c r="L147">
         <v>8</v>
       </c>
-    </row>
-    <row r="148" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M147" t="s">
+        <v>343</v>
+      </c>
+      <c r="N147" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="148" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B148" t="s">
         <v>330</v>
       </c>
@@ -7319,8 +7932,14 @@
       <c r="L148">
         <v>8</v>
       </c>
-    </row>
-    <row r="149" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M148" t="s">
+        <v>343</v>
+      </c>
+      <c r="N148" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="149" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B149" t="s">
         <v>330</v>
       </c>
@@ -7354,8 +7973,14 @@
       <c r="L149">
         <v>8</v>
       </c>
-    </row>
-    <row r="150" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M149" t="s">
+        <v>343</v>
+      </c>
+      <c r="N149" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="150" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B150" t="s">
         <v>330</v>
       </c>
@@ -7389,8 +8014,14 @@
       <c r="L150">
         <v>8</v>
       </c>
-    </row>
-    <row r="151" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M150" t="s">
+        <v>343</v>
+      </c>
+      <c r="N150" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="151" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B151" t="s">
         <v>330</v>
       </c>
@@ -7424,8 +8055,14 @@
       <c r="L151">
         <v>8</v>
       </c>
-    </row>
-    <row r="152" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M151" t="s">
+        <v>343</v>
+      </c>
+      <c r="N151" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="152" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B152" t="s">
         <v>330</v>
       </c>
@@ -7459,8 +8096,14 @@
       <c r="L152">
         <v>8</v>
       </c>
-    </row>
-    <row r="153" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M152" t="s">
+        <v>343</v>
+      </c>
+      <c r="N152" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="153" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B153" t="s">
         <v>330</v>
       </c>
@@ -7494,8 +8137,14 @@
       <c r="L153">
         <v>8</v>
       </c>
-    </row>
-    <row r="154" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M153" t="s">
+        <v>343</v>
+      </c>
+      <c r="N153" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="154" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B154" t="s">
         <v>330</v>
       </c>
@@ -7529,8 +8178,14 @@
       <c r="L154">
         <v>8</v>
       </c>
-    </row>
-    <row r="155" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M154" t="s">
+        <v>343</v>
+      </c>
+      <c r="N154" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="155" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B155" t="s">
         <v>330</v>
       </c>
@@ -7564,8 +8219,14 @@
       <c r="L155">
         <v>8</v>
       </c>
-    </row>
-    <row r="156" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M155" t="s">
+        <v>343</v>
+      </c>
+      <c r="N155" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="156" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B156" t="s">
         <v>335</v>
       </c>
@@ -7599,8 +8260,14 @@
       <c r="L156">
         <v>16</v>
       </c>
-    </row>
-    <row r="157" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M156" t="s">
+        <v>347</v>
+      </c>
+      <c r="N156" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="157" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B157" t="s">
         <v>334</v>
       </c>
@@ -7634,8 +8301,14 @@
       <c r="L157">
         <v>51</v>
       </c>
-    </row>
-    <row r="158" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M157" t="s">
+        <v>347</v>
+      </c>
+      <c r="N157" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="158" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B158" t="s">
         <v>330</v>
       </c>
@@ -7669,8 +8342,14 @@
       <c r="L158">
         <v>69</v>
       </c>
-    </row>
-    <row r="159" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M158" t="s">
+        <v>360</v>
+      </c>
+      <c r="N158" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="159" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B159" t="s">
         <v>335</v>
       </c>
@@ -7704,8 +8383,14 @@
       <c r="L159">
         <v>18</v>
       </c>
-    </row>
-    <row r="160" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M159" t="s">
+        <v>364</v>
+      </c>
+      <c r="N159" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="160" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B160" t="s">
         <v>331</v>
       </c>
@@ -7739,8 +8424,14 @@
       <c r="L160">
         <v>62</v>
       </c>
-    </row>
-    <row r="161" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M160" t="s">
+        <v>342</v>
+      </c>
+      <c r="N160" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="161" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B161" t="s">
         <v>331</v>
       </c>
@@ -7774,8 +8465,14 @@
       <c r="L161">
         <v>42</v>
       </c>
-    </row>
-    <row r="162" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M161" t="s">
+        <v>342</v>
+      </c>
+      <c r="N161" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="162" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B162" t="s">
         <v>331</v>
       </c>
@@ -7809,8 +8506,14 @@
       <c r="L162">
         <v>23</v>
       </c>
-    </row>
-    <row r="163" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M162" t="s">
+        <v>342</v>
+      </c>
+      <c r="N162" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="163" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B163" t="s">
         <v>331</v>
       </c>
@@ -7844,8 +8547,14 @@
       <c r="L163">
         <v>34</v>
       </c>
-    </row>
-    <row r="164" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M163" t="s">
+        <v>342</v>
+      </c>
+      <c r="N163" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="164" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B164" t="s">
         <v>331</v>
       </c>
@@ -7879,8 +8588,14 @@
       <c r="L164">
         <v>43</v>
       </c>
-    </row>
-    <row r="165" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M164" t="s">
+        <v>342</v>
+      </c>
+      <c r="N164" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="165" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B165" t="s">
         <v>331</v>
       </c>
@@ -7914,8 +8629,14 @@
       <c r="L165">
         <v>39</v>
       </c>
-    </row>
-    <row r="166" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M165" t="s">
+        <v>342</v>
+      </c>
+      <c r="N165" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="166" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B166" t="s">
         <v>331</v>
       </c>
@@ -7949,8 +8670,14 @@
       <c r="L166">
         <v>45</v>
       </c>
-    </row>
-    <row r="167" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M166" t="s">
+        <v>342</v>
+      </c>
+      <c r="N166" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="167" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B167" t="s">
         <v>331</v>
       </c>
@@ -7984,8 +8711,14 @@
       <c r="L167">
         <v>40</v>
       </c>
-    </row>
-    <row r="168" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M167" t="s">
+        <v>342</v>
+      </c>
+      <c r="N167" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="168" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B168" t="s">
         <v>331</v>
       </c>
@@ -8020,7 +8753,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="169" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B169" t="s">
         <v>331</v>
       </c>
@@ -8055,7 +8788,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="170" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B170" t="s">
         <v>331</v>
       </c>
@@ -8089,8 +8822,14 @@
       <c r="L170">
         <v>42</v>
       </c>
-    </row>
-    <row r="171" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M170" t="s">
+        <v>342</v>
+      </c>
+      <c r="N170" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="171" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B171" t="s">
         <v>331</v>
       </c>
@@ -8124,8 +8863,14 @@
       <c r="L171">
         <v>42</v>
       </c>
-    </row>
-    <row r="172" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M171" t="s">
+        <v>342</v>
+      </c>
+      <c r="N171" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="172" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B172" t="s">
         <v>335</v>
       </c>
@@ -8160,7 +8905,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="173" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="173" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B173" t="s">
         <v>335</v>
       </c>
@@ -8195,7 +8940,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="174" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="174" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B174" t="s">
         <v>335</v>
       </c>
@@ -8230,7 +8975,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="175" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B175" t="s">
         <v>331</v>
       </c>
@@ -8264,8 +9009,14 @@
       <c r="L175">
         <v>95</v>
       </c>
-    </row>
-    <row r="176" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M175" t="s">
+        <v>342</v>
+      </c>
+      <c r="N175" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="176" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B176" t="s">
         <v>330</v>
       </c>
@@ -8299,8 +9050,14 @@
       <c r="L176">
         <v>12</v>
       </c>
-    </row>
-    <row r="177" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M176" t="s">
+        <v>339</v>
+      </c>
+      <c r="N176" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="177" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B177" t="s">
         <v>331</v>
       </c>
@@ -8334,8 +9091,14 @@
       <c r="L177">
         <v>19</v>
       </c>
-    </row>
-    <row r="178" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M177" t="s">
+        <v>357</v>
+      </c>
+      <c r="N177" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="178" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B178" t="s">
         <v>331</v>
       </c>
@@ -8369,8 +9132,14 @@
       <c r="L178">
         <v>20</v>
       </c>
-    </row>
-    <row r="179" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M178" t="s">
+        <v>357</v>
+      </c>
+      <c r="N178" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="179" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B179" t="s">
         <v>331</v>
       </c>
@@ -8404,8 +9173,14 @@
       <c r="L179">
         <v>76</v>
       </c>
-    </row>
-    <row r="180" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M179" t="s">
+        <v>342</v>
+      </c>
+      <c r="N179" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="180" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B180" t="s">
         <v>331</v>
       </c>
@@ -8439,8 +9214,14 @@
       <c r="L180">
         <v>70</v>
       </c>
-    </row>
-    <row r="181" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M180" t="s">
+        <v>342</v>
+      </c>
+      <c r="N180" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="181" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B181" t="s">
         <v>331</v>
       </c>
@@ -8474,8 +9255,14 @@
       <c r="L181">
         <v>82</v>
       </c>
-    </row>
-    <row r="182" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M181" t="s">
+        <v>342</v>
+      </c>
+      <c r="N181" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="182" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B182" t="s">
         <v>331</v>
       </c>
@@ -8509,8 +9296,14 @@
       <c r="L182">
         <v>76</v>
       </c>
-    </row>
-    <row r="183" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M182" t="s">
+        <v>342</v>
+      </c>
+      <c r="N182" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="183" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B183" t="s">
         <v>331</v>
       </c>
@@ -8544,8 +9337,14 @@
       <c r="L183">
         <v>68</v>
       </c>
-    </row>
-    <row r="184" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M183" t="s">
+        <v>342</v>
+      </c>
+      <c r="N183" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="184" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B184" t="s">
         <v>332</v>
       </c>
@@ -8580,7 +9379,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="185" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="185" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B185" t="s">
         <v>332</v>
       </c>
@@ -8615,7 +9414,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="186" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="186" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B186" t="s">
         <v>332</v>
       </c>
@@ -8650,7 +9449,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="187" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="187" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B187" t="s">
         <v>332</v>
       </c>
@@ -8685,7 +9484,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="188" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="188" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B188" t="s">
         <v>332</v>
       </c>
@@ -8720,7 +9519,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="189" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="189" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B189" t="s">
         <v>332</v>
       </c>
@@ -8755,7 +9554,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="190" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="190" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B190" t="s">
         <v>332</v>
       </c>
@@ -8790,7 +9589,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="191" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="191" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B191" t="s">
         <v>332</v>
       </c>
@@ -8825,7 +9624,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="192" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="192" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B192" t="s">
         <v>331</v>
       </c>
@@ -8859,8 +9658,14 @@
       <c r="L192">
         <v>67</v>
       </c>
-    </row>
-    <row r="193" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M192" t="s">
+        <v>342</v>
+      </c>
+      <c r="N192" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="193" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B193" t="s">
         <v>331</v>
       </c>
@@ -8894,8 +9699,14 @@
       <c r="L193">
         <v>38</v>
       </c>
-    </row>
-    <row r="194" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M193" t="s">
+        <v>342</v>
+      </c>
+      <c r="N193" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="194" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B194" t="s">
         <v>331</v>
       </c>
@@ -8929,8 +9740,14 @@
       <c r="L194">
         <v>52</v>
       </c>
-    </row>
-    <row r="195" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M194" t="s">
+        <v>342</v>
+      </c>
+      <c r="N194" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="195" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B195" t="s">
         <v>331</v>
       </c>
@@ -8964,8 +9781,14 @@
       <c r="L195">
         <v>36</v>
       </c>
-    </row>
-    <row r="196" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M195" t="s">
+        <v>342</v>
+      </c>
+      <c r="N195" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="196" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B196" t="s">
         <v>331</v>
       </c>
@@ -8999,8 +9822,14 @@
       <c r="L196">
         <v>25</v>
       </c>
-    </row>
-    <row r="197" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M196" t="s">
+        <v>342</v>
+      </c>
+      <c r="N196" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="197" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B197" t="s">
         <v>331</v>
       </c>
@@ -9034,8 +9863,14 @@
       <c r="L197">
         <v>60</v>
       </c>
-    </row>
-    <row r="198" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M197" t="s">
+        <v>342</v>
+      </c>
+      <c r="N197" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="198" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B198" t="s">
         <v>331</v>
       </c>
@@ -9069,8 +9904,14 @@
       <c r="L198">
         <v>47</v>
       </c>
-    </row>
-    <row r="199" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M198" t="s">
+        <v>342</v>
+      </c>
+      <c r="N198" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="199" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B199" t="s">
         <v>331</v>
       </c>
@@ -9104,8 +9945,14 @@
       <c r="L199">
         <v>51</v>
       </c>
-    </row>
-    <row r="200" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M199" t="s">
+        <v>342</v>
+      </c>
+      <c r="N199" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="200" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B200" t="s">
         <v>331</v>
       </c>
@@ -9139,8 +9986,14 @@
       <c r="L200">
         <v>52</v>
       </c>
-    </row>
-    <row r="201" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M200" t="s">
+        <v>342</v>
+      </c>
+      <c r="N200" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="201" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B201" t="s">
         <v>331</v>
       </c>
@@ -9174,8 +10027,14 @@
       <c r="L201">
         <v>56</v>
       </c>
-    </row>
-    <row r="202" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M201" t="s">
+        <v>342</v>
+      </c>
+      <c r="N201" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="202" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B202" t="s">
         <v>331</v>
       </c>
@@ -9209,8 +10068,14 @@
       <c r="L202">
         <v>51</v>
       </c>
-    </row>
-    <row r="203" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M202" t="s">
+        <v>342</v>
+      </c>
+      <c r="N202" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="203" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B203" t="s">
         <v>331</v>
       </c>
@@ -9244,8 +10109,14 @@
       <c r="L203">
         <v>43</v>
       </c>
-    </row>
-    <row r="204" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M203" t="s">
+        <v>342</v>
+      </c>
+      <c r="N203" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="204" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B204" t="s">
         <v>331</v>
       </c>
@@ -9279,8 +10150,14 @@
       <c r="L204">
         <v>45</v>
       </c>
-    </row>
-    <row r="205" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M204" t="s">
+        <v>342</v>
+      </c>
+      <c r="N204" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="205" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B205" t="s">
         <v>331</v>
       </c>
@@ -9314,8 +10191,14 @@
       <c r="L205">
         <v>78</v>
       </c>
-    </row>
-    <row r="206" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M205" t="s">
+        <v>342</v>
+      </c>
+      <c r="N205" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="206" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B206" t="s">
         <v>331</v>
       </c>
@@ -9349,8 +10232,14 @@
       <c r="L206">
         <v>52</v>
       </c>
-    </row>
-    <row r="207" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M206" t="s">
+        <v>342</v>
+      </c>
+      <c r="N206" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="207" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B207" t="s">
         <v>331</v>
       </c>
@@ -9384,8 +10273,14 @@
       <c r="L207">
         <v>81</v>
       </c>
-    </row>
-    <row r="208" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M207" t="s">
+        <v>342</v>
+      </c>
+      <c r="N207" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="208" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B208" t="s">
         <v>331</v>
       </c>
@@ -9419,8 +10314,14 @@
       <c r="L208">
         <v>40</v>
       </c>
-    </row>
-    <row r="209" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M208" t="s">
+        <v>342</v>
+      </c>
+      <c r="N208" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="209" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B209" t="s">
         <v>331</v>
       </c>
@@ -9454,8 +10355,14 @@
       <c r="L209">
         <v>54</v>
       </c>
-    </row>
-    <row r="210" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M209" t="s">
+        <v>342</v>
+      </c>
+      <c r="N209" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="210" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B210" t="s">
         <v>331</v>
       </c>
@@ -9489,8 +10396,14 @@
       <c r="L210">
         <v>46</v>
       </c>
-    </row>
-    <row r="211" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M210" t="s">
+        <v>342</v>
+      </c>
+      <c r="N210" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="211" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B211" t="s">
         <v>331</v>
       </c>
@@ -9524,8 +10437,14 @@
       <c r="L211">
         <v>44</v>
       </c>
-    </row>
-    <row r="212" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M211" t="s">
+        <v>342</v>
+      </c>
+      <c r="N211" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="212" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B212" t="s">
         <v>331</v>
       </c>
@@ -9559,8 +10478,14 @@
       <c r="L212">
         <v>44</v>
       </c>
-    </row>
-    <row r="213" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M212" t="s">
+        <v>342</v>
+      </c>
+      <c r="N212" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="213" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B213" t="s">
         <v>331</v>
       </c>
@@ -9594,8 +10519,14 @@
       <c r="L213">
         <v>35</v>
       </c>
-    </row>
-    <row r="214" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M213" t="s">
+        <v>342</v>
+      </c>
+      <c r="N213" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="214" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B214" t="s">
         <v>331</v>
       </c>
@@ -9629,8 +10560,14 @@
       <c r="L214">
         <v>26</v>
       </c>
-    </row>
-    <row r="215" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M214" t="s">
+        <v>342</v>
+      </c>
+      <c r="N214" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="215" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B215" t="s">
         <v>331</v>
       </c>
@@ -9664,8 +10601,14 @@
       <c r="L215">
         <v>78</v>
       </c>
-    </row>
-    <row r="216" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M215" t="s">
+        <v>342</v>
+      </c>
+      <c r="N215" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="216" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B216" t="s">
         <v>331</v>
       </c>
@@ -9699,8 +10642,14 @@
       <c r="L216">
         <v>56</v>
       </c>
-    </row>
-    <row r="217" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M216" t="s">
+        <v>342</v>
+      </c>
+      <c r="N216" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="217" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B217" t="s">
         <v>331</v>
       </c>
@@ -9734,8 +10683,14 @@
       <c r="L217">
         <v>46</v>
       </c>
-    </row>
-    <row r="218" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M217" t="s">
+        <v>342</v>
+      </c>
+      <c r="N217" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="218" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B218" t="s">
         <v>331</v>
       </c>
@@ -9770,7 +10725,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="219" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="219" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B219" t="s">
         <v>331</v>
       </c>
@@ -9804,8 +10759,14 @@
       <c r="L219">
         <v>46</v>
       </c>
-    </row>
-    <row r="220" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M219" t="s">
+        <v>342</v>
+      </c>
+      <c r="N219" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="220" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B220" t="s">
         <v>331</v>
       </c>
@@ -9839,8 +10800,14 @@
       <c r="L220">
         <v>40</v>
       </c>
-    </row>
-    <row r="221" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M220" t="s">
+        <v>342</v>
+      </c>
+      <c r="N220" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="221" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B221" t="s">
         <v>331</v>
       </c>
@@ -9874,8 +10841,14 @@
       <c r="L221">
         <v>29</v>
       </c>
-    </row>
-    <row r="222" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M221" t="s">
+        <v>342</v>
+      </c>
+      <c r="N221" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="222" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B222" t="s">
         <v>331</v>
       </c>
@@ -9909,8 +10882,14 @@
       <c r="L222">
         <v>28</v>
       </c>
-    </row>
-    <row r="223" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M222" t="s">
+        <v>342</v>
+      </c>
+      <c r="N222" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="223" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B223" t="s">
         <v>331</v>
       </c>
@@ -9944,8 +10923,14 @@
       <c r="L223">
         <v>58</v>
       </c>
-    </row>
-    <row r="224" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M223" t="s">
+        <v>342</v>
+      </c>
+      <c r="N223" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="224" spans="2:14" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B224" t="s">
         <v>330</v>
       </c>

</xml_diff>